<commit_message>
orange staff and purple staff finish
</commit_message>
<xml_diff>
--- a/多功能武器策划记事.xlsx
+++ b/多功能武器策划记事.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13545" windowHeight="12375"/>
+    <workbookView windowWidth="27945" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="武器功能及对应 tag、组件" sheetId="1" r:id="rId1"/>
@@ -749,7 +749,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -764,6 +764,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1293,12 +1299,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -1415,8 +1421,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1428,16 +1434,11 @@
       <c r="D8" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
@@ -1446,23 +1447,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="5:5">
-      <c r="E11" s="2" t="s">
+    <row r="12" spans="5:5">
+      <c r="E12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>